<commit_message>
More work on making graphs update automatically
</commit_message>
<xml_diff>
--- a/Charger_Cycle_Performance.xlsx
+++ b/Charger_Cycle_Performance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\Dropbox\GitHub\ChargerBatteryCyclePerformance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75B6127C-177D-4162-BE6A-25EF1A7E76AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46BC3317-0963-47AD-9275-01DC98351431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B9646992-58BC-44A8-9040-42DC40CCACD9}"/>
   </bookViews>
@@ -23,6 +23,11 @@
     <definedName name="_LH2">OFFSET(Report!$O$38,0,0,Report!$O$33,1)</definedName>
     <definedName name="_LT1">OFFSET(Report!$L$38,0,0,Report!$L$33,1)</definedName>
     <definedName name="_LT2">OFFSET(Report!$M$38,0,0,Report!$M$33,1)</definedName>
+    <definedName name="_TFW1">OFFSET(Report!$H$38,0,0,Report!$J$33,1)</definedName>
+    <definedName name="_TFW2">OFFSET(Report!$H$38,0,0,Report!$K$33,1)</definedName>
+    <definedName name="_TLT1">OFFSET(Report!$H$38,0,0,Report!$M$33,1)</definedName>
+    <definedName name="_TLT2">OFFSET(Report!$H$38,0,0,Report!$M$33,1)</definedName>
+    <definedName name="_TVN">OFFSET(Report!$H$38,0,0,Report!$I$33,1)</definedName>
     <definedName name="_VN1">OFFSET(Report!$I$38,0,0,Report!$I$33,1)</definedName>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">Report!$B$37:$E$1165</definedName>
   </definedNames>
@@ -98,7 +103,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -503,776 +508,395 @@
             </c:spPr>
           </c:marker>
           <c:xVal>
-            <c:multiLvlStrRef>
-              <c:f>Report!$H$38:$I$163</c:f>
-              <c:multiLvlStrCache>
+            <c:numRef>
+              <c:f>[0]!_TVN</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="126"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>#N/A</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>#N/A</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>#N/A</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>#N/A</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>#N/A</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>#N/A</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>#N/A</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>#N/A</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>0.995525288</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>0.993648091</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>0.995721738</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>1</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>0.997970009</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>0.998843123</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>0.995307009</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>0.998755812</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>0.997598935</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>0.99508873</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v>0.993669919</c:v>
-                  </c:pt>
-                  <c:pt idx="19">
-                    <c:v>0.99805732</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>0.996398402</c:v>
-                  </c:pt>
-                  <c:pt idx="21">
-                    <c:v>0.992862288</c:v>
-                  </c:pt>
-                  <c:pt idx="22">
-                    <c:v>0.997729902</c:v>
-                  </c:pt>
-                  <c:pt idx="23">
-                    <c:v>0.993800886</c:v>
-                  </c:pt>
-                  <c:pt idx="24">
-                    <c:v>0.99314605</c:v>
-                  </c:pt>
-                  <c:pt idx="25">
-                    <c:v>0.992884116</c:v>
-                  </c:pt>
-                  <c:pt idx="26">
-                    <c:v>0.995285181</c:v>
-                  </c:pt>
-                  <c:pt idx="27">
-                    <c:v>0.995612599</c:v>
-                  </c:pt>
-                  <c:pt idx="28">
-                    <c:v>0.995481632</c:v>
-                  </c:pt>
-                  <c:pt idx="29">
-                    <c:v>0.995743566</c:v>
-                  </c:pt>
-                  <c:pt idx="30">
-                    <c:v>0.993298845</c:v>
-                  </c:pt>
-                  <c:pt idx="31">
-                    <c:v>0.992971427</c:v>
-                  </c:pt>
-                  <c:pt idx="32">
-                    <c:v>0.993931853</c:v>
-                  </c:pt>
-                  <c:pt idx="33">
-                    <c:v>0.994106476</c:v>
-                  </c:pt>
-                  <c:pt idx="34">
-                    <c:v>0.992774977</c:v>
-                  </c:pt>
-                  <c:pt idx="35">
-                    <c:v>0.993102395</c:v>
-                  </c:pt>
-                  <c:pt idx="36">
-                    <c:v>0.991989173</c:v>
-                  </c:pt>
-                  <c:pt idx="37">
-                    <c:v>0.990570362</c:v>
-                  </c:pt>
-                  <c:pt idx="38">
-                    <c:v>0.992687665</c:v>
-                  </c:pt>
-                  <c:pt idx="39">
-                    <c:v>0.987972846</c:v>
-                  </c:pt>
-                  <c:pt idx="40">
-                    <c:v>0.988540371</c:v>
-                  </c:pt>
-                  <c:pt idx="41">
-                    <c:v>0.989391657</c:v>
-                  </c:pt>
-                  <c:pt idx="42">
-                    <c:v>0.986728658</c:v>
-                  </c:pt>
-                  <c:pt idx="43">
-                    <c:v>0.987558117</c:v>
-                  </c:pt>
-                  <c:pt idx="44">
-                    <c:v>0.990614018</c:v>
-                  </c:pt>
-                  <c:pt idx="45">
-                    <c:v>0.990330256</c:v>
-                  </c:pt>
-                  <c:pt idx="46">
-                    <c:v>0.989217034</c:v>
-                  </c:pt>
-                  <c:pt idx="47">
-                    <c:v>0.990395739</c:v>
-                  </c:pt>
-                  <c:pt idx="48">
-                    <c:v>0.991028747</c:v>
-                  </c:pt>
-                  <c:pt idx="49">
-                    <c:v>0.989129723</c:v>
-                  </c:pt>
-                  <c:pt idx="50">
-                    <c:v>0.990657674</c:v>
-                  </c:pt>
-                  <c:pt idx="51">
-                    <c:v>0.989217034</c:v>
-                  </c:pt>
-                  <c:pt idx="52">
-                    <c:v>0.986750486</c:v>
-                  </c:pt>
-                  <c:pt idx="53">
-                    <c:v>0.987099732</c:v>
-                  </c:pt>
-                  <c:pt idx="54">
-                    <c:v>0.985309847</c:v>
-                  </c:pt>
-                  <c:pt idx="55">
-                    <c:v>0.981162552</c:v>
-                  </c:pt>
-                  <c:pt idx="56">
-                    <c:v>0.98312706</c:v>
-                  </c:pt>
-                  <c:pt idx="57">
-                    <c:v>0.986226617</c:v>
-                  </c:pt>
-                  <c:pt idx="58">
-                    <c:v>0.984109314</c:v>
-                  </c:pt>
-                  <c:pt idx="59">
-                    <c:v>0.985418986</c:v>
-                  </c:pt>
-                  <c:pt idx="60">
-                    <c:v>0.982472224</c:v>
-                  </c:pt>
-                  <c:pt idx="61">
-                    <c:v>0.988387576</c:v>
-                  </c:pt>
-                  <c:pt idx="62">
-                    <c:v>0.983017921</c:v>
-                  </c:pt>
-                  <c:pt idx="63">
-                    <c:v>0.984698666</c:v>
-                  </c:pt>
-                  <c:pt idx="64">
-                    <c:v>0.982363085</c:v>
-                  </c:pt>
-                  <c:pt idx="65">
-                    <c:v>0.981446314</c:v>
-                  </c:pt>
-                  <c:pt idx="66">
-                    <c:v>0.980747823</c:v>
-                  </c:pt>
-                  <c:pt idx="67">
-                    <c:v>0.977146225</c:v>
-                  </c:pt>
-                  <c:pt idx="68">
-                    <c:v>0.979569118</c:v>
-                  </c:pt>
-                  <c:pt idx="69">
-                    <c:v>0.978608692</c:v>
-                  </c:pt>
-                  <c:pt idx="70">
-                    <c:v>0.980223954</c:v>
-                  </c:pt>
-                  <c:pt idx="71">
-                    <c:v>0.980987929</c:v>
-                  </c:pt>
-                  <c:pt idx="72">
-                    <c:v>0.984262109</c:v>
-                  </c:pt>
-                  <c:pt idx="73">
-                    <c:v>0.980333093</c:v>
-                  </c:pt>
-                  <c:pt idx="74">
-                    <c:v>0.978761487</c:v>
-                  </c:pt>
-                  <c:pt idx="75">
-                    <c:v>0.978499553</c:v>
-                  </c:pt>
-                  <c:pt idx="76">
-                    <c:v>0.982734158</c:v>
-                  </c:pt>
-                  <c:pt idx="77">
-                    <c:v>0.981577282</c:v>
-                  </c:pt>
-                  <c:pt idx="78">
-                    <c:v>0.98087879</c:v>
-                  </c:pt>
-                  <c:pt idx="79">
-                    <c:v>0.98240674</c:v>
-                  </c:pt>
-                  <c:pt idx="80">
-                    <c:v>0.977975684</c:v>
-                  </c:pt>
-                  <c:pt idx="81">
-                    <c:v>0.978041167</c:v>
-                  </c:pt>
-                  <c:pt idx="82">
-                    <c:v>0.981140724</c:v>
-                  </c:pt>
-                  <c:pt idx="83">
-                    <c:v>0.972911619</c:v>
-                  </c:pt>
-                  <c:pt idx="84">
-                    <c:v>0.979634602</c:v>
-                  </c:pt>
-                  <c:pt idx="85">
-                    <c:v>0.974264947</c:v>
-                  </c:pt>
-                  <c:pt idx="86">
-                    <c:v>0.973064414</c:v>
-                  </c:pt>
-                  <c:pt idx="87">
-                    <c:v>0.975007094</c:v>
-                  </c:pt>
-                  <c:pt idx="88">
-                    <c:v>0.975771069</c:v>
-                  </c:pt>
-                  <c:pt idx="89">
-                    <c:v>0.974701504</c:v>
-                  </c:pt>
-                  <c:pt idx="90">
-                    <c:v>0.973806561</c:v>
-                  </c:pt>
-                  <c:pt idx="91">
-                    <c:v>0.976556873</c:v>
-                  </c:pt>
-                  <c:pt idx="92">
-                    <c:v>0.975247201</c:v>
-                  </c:pt>
-                  <c:pt idx="93">
-                    <c:v>0.974046668</c:v>
-                  </c:pt>
-                  <c:pt idx="94">
-                    <c:v>0.975945692</c:v>
-                  </c:pt>
-                  <c:pt idx="95">
-                    <c:v>0.971885709</c:v>
-                  </c:pt>
-                  <c:pt idx="96">
-                    <c:v>0.973762906</c:v>
-                  </c:pt>
-                  <c:pt idx="97">
-                    <c:v>0.970685177</c:v>
-                  </c:pt>
-                  <c:pt idx="98">
-                    <c:v>0.970248619</c:v>
-                  </c:pt>
-                  <c:pt idx="99">
-                    <c:v>0.969746578</c:v>
-                  </c:pt>
-                  <c:pt idx="100">
-                    <c:v>0.970095824</c:v>
-                  </c:pt>
-                  <c:pt idx="101">
-                    <c:v>0.968829808</c:v>
-                  </c:pt>
-                  <c:pt idx="102">
-                    <c:v>0.96697444</c:v>
-                  </c:pt>
-                  <c:pt idx="103">
-                    <c:v>0.966603366</c:v>
-                  </c:pt>
-                  <c:pt idx="104">
-                    <c:v>0.968305939</c:v>
-                  </c:pt>
-                  <c:pt idx="105">
-                    <c:v>0.968305939</c:v>
-                  </c:pt>
-                  <c:pt idx="106">
-                    <c:v>0.967934866</c:v>
-                  </c:pt>
-                  <c:pt idx="107">
-                    <c:v>0.967258202</c:v>
-                  </c:pt>
-                  <c:pt idx="108">
-                    <c:v>0.965861218</c:v>
-                  </c:pt>
-                  <c:pt idx="109">
-                    <c:v>0.965730251</c:v>
-                  </c:pt>
-                  <c:pt idx="110">
-                    <c:v>0.966734333</c:v>
-                  </c:pt>
-                  <c:pt idx="111">
-                    <c:v>0.965752079</c:v>
-                  </c:pt>
-                  <c:pt idx="112">
-                    <c:v>0.965359178</c:v>
-                  </c:pt>
-                  <c:pt idx="113">
-                    <c:v>0.965992186</c:v>
-                  </c:pt>
-                  <c:pt idx="114">
-                    <c:v>0.964289612</c:v>
-                  </c:pt>
-                  <c:pt idx="115">
-                    <c:v>0.963787571</c:v>
-                  </c:pt>
-                  <c:pt idx="116">
-                    <c:v>0.964551547</c:v>
-                  </c:pt>
-                  <c:pt idx="117">
-                    <c:v>0.965773907</c:v>
-                  </c:pt>
-                  <c:pt idx="118">
-                    <c:v>0.96400585</c:v>
-                  </c:pt>
-                  <c:pt idx="119">
-                    <c:v>0.964049506</c:v>
-                  </c:pt>
-                  <c:pt idx="120">
-                    <c:v>0.961604785</c:v>
-                  </c:pt>
-                  <c:pt idx="121">
-                    <c:v>0.965664768</c:v>
-                  </c:pt>
-                  <c:pt idx="122">
-                    <c:v>0.965817563</c:v>
-                  </c:pt>
-                  <c:pt idx="123">
-                    <c:v>0.963351014</c:v>
-                  </c:pt>
-                  <c:pt idx="124">
-                    <c:v>0.96697444</c:v>
-                  </c:pt>
-                  <c:pt idx="125">
-                    <c:v>0.961364678</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>1</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>2</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>3</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>4</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>5</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>6</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>7</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>8</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>9</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>10</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>11</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>12</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>13</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>14</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>15</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>16</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>17</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>18</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v>19</c:v>
-                  </c:pt>
-                  <c:pt idx="19">
-                    <c:v>20</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>21</c:v>
-                  </c:pt>
-                  <c:pt idx="21">
-                    <c:v>22</c:v>
-                  </c:pt>
-                  <c:pt idx="22">
-                    <c:v>23</c:v>
-                  </c:pt>
-                  <c:pt idx="23">
-                    <c:v>24</c:v>
-                  </c:pt>
-                  <c:pt idx="24">
-                    <c:v>25</c:v>
-                  </c:pt>
-                  <c:pt idx="25">
-                    <c:v>26</c:v>
-                  </c:pt>
-                  <c:pt idx="26">
-                    <c:v>27</c:v>
-                  </c:pt>
-                  <c:pt idx="27">
-                    <c:v>28</c:v>
-                  </c:pt>
-                  <c:pt idx="28">
-                    <c:v>29</c:v>
-                  </c:pt>
-                  <c:pt idx="29">
-                    <c:v>30</c:v>
-                  </c:pt>
-                  <c:pt idx="30">
-                    <c:v>31</c:v>
-                  </c:pt>
-                  <c:pt idx="31">
-                    <c:v>32</c:v>
-                  </c:pt>
-                  <c:pt idx="32">
-                    <c:v>33</c:v>
-                  </c:pt>
-                  <c:pt idx="33">
-                    <c:v>34</c:v>
-                  </c:pt>
-                  <c:pt idx="34">
-                    <c:v>35</c:v>
-                  </c:pt>
-                  <c:pt idx="35">
-                    <c:v>36</c:v>
-                  </c:pt>
-                  <c:pt idx="36">
-                    <c:v>37</c:v>
-                  </c:pt>
-                  <c:pt idx="37">
-                    <c:v>38</c:v>
-                  </c:pt>
-                  <c:pt idx="38">
-                    <c:v>39</c:v>
-                  </c:pt>
-                  <c:pt idx="39">
-                    <c:v>40</c:v>
-                  </c:pt>
-                  <c:pt idx="40">
-                    <c:v>41</c:v>
-                  </c:pt>
-                  <c:pt idx="41">
-                    <c:v>42</c:v>
-                  </c:pt>
-                  <c:pt idx="42">
-                    <c:v>43</c:v>
-                  </c:pt>
-                  <c:pt idx="43">
-                    <c:v>44</c:v>
-                  </c:pt>
-                  <c:pt idx="44">
-                    <c:v>45</c:v>
-                  </c:pt>
-                  <c:pt idx="45">
-                    <c:v>46</c:v>
-                  </c:pt>
-                  <c:pt idx="46">
-                    <c:v>47</c:v>
-                  </c:pt>
-                  <c:pt idx="47">
-                    <c:v>48</c:v>
-                  </c:pt>
-                  <c:pt idx="48">
-                    <c:v>49</c:v>
-                  </c:pt>
-                  <c:pt idx="49">
-                    <c:v>50</c:v>
-                  </c:pt>
-                  <c:pt idx="50">
-                    <c:v>51</c:v>
-                  </c:pt>
-                  <c:pt idx="51">
-                    <c:v>52</c:v>
-                  </c:pt>
-                  <c:pt idx="52">
-                    <c:v>53</c:v>
-                  </c:pt>
-                  <c:pt idx="53">
-                    <c:v>54</c:v>
-                  </c:pt>
-                  <c:pt idx="54">
-                    <c:v>55</c:v>
-                  </c:pt>
-                  <c:pt idx="55">
-                    <c:v>56</c:v>
-                  </c:pt>
-                  <c:pt idx="56">
-                    <c:v>57</c:v>
-                  </c:pt>
-                  <c:pt idx="57">
-                    <c:v>58</c:v>
-                  </c:pt>
-                  <c:pt idx="58">
-                    <c:v>59</c:v>
-                  </c:pt>
-                  <c:pt idx="59">
-                    <c:v>60</c:v>
-                  </c:pt>
-                  <c:pt idx="60">
-                    <c:v>61</c:v>
-                  </c:pt>
-                  <c:pt idx="61">
-                    <c:v>62</c:v>
-                  </c:pt>
-                  <c:pt idx="62">
-                    <c:v>63</c:v>
-                  </c:pt>
-                  <c:pt idx="63">
-                    <c:v>64</c:v>
-                  </c:pt>
-                  <c:pt idx="64">
-                    <c:v>65</c:v>
-                  </c:pt>
-                  <c:pt idx="65">
-                    <c:v>66</c:v>
-                  </c:pt>
-                  <c:pt idx="66">
-                    <c:v>67</c:v>
-                  </c:pt>
-                  <c:pt idx="67">
-                    <c:v>68</c:v>
-                  </c:pt>
-                  <c:pt idx="68">
-                    <c:v>69</c:v>
-                  </c:pt>
-                  <c:pt idx="69">
-                    <c:v>70</c:v>
-                  </c:pt>
-                  <c:pt idx="70">
-                    <c:v>71</c:v>
-                  </c:pt>
-                  <c:pt idx="71">
-                    <c:v>72</c:v>
-                  </c:pt>
-                  <c:pt idx="72">
-                    <c:v>73</c:v>
-                  </c:pt>
-                  <c:pt idx="73">
-                    <c:v>74</c:v>
-                  </c:pt>
-                  <c:pt idx="74">
-                    <c:v>75</c:v>
-                  </c:pt>
-                  <c:pt idx="75">
-                    <c:v>76</c:v>
-                  </c:pt>
-                  <c:pt idx="76">
-                    <c:v>77</c:v>
-                  </c:pt>
-                  <c:pt idx="77">
-                    <c:v>78</c:v>
-                  </c:pt>
-                  <c:pt idx="78">
-                    <c:v>79</c:v>
-                  </c:pt>
-                  <c:pt idx="79">
-                    <c:v>80</c:v>
-                  </c:pt>
-                  <c:pt idx="80">
-                    <c:v>81</c:v>
-                  </c:pt>
-                  <c:pt idx="81">
-                    <c:v>82</c:v>
-                  </c:pt>
-                  <c:pt idx="82">
-                    <c:v>83</c:v>
-                  </c:pt>
-                  <c:pt idx="83">
-                    <c:v>84</c:v>
-                  </c:pt>
-                  <c:pt idx="84">
-                    <c:v>85</c:v>
-                  </c:pt>
-                  <c:pt idx="85">
-                    <c:v>86</c:v>
-                  </c:pt>
-                  <c:pt idx="86">
-                    <c:v>87</c:v>
-                  </c:pt>
-                  <c:pt idx="87">
-                    <c:v>88</c:v>
-                  </c:pt>
-                  <c:pt idx="88">
-                    <c:v>89</c:v>
-                  </c:pt>
-                  <c:pt idx="89">
-                    <c:v>90</c:v>
-                  </c:pt>
-                  <c:pt idx="90">
-                    <c:v>91</c:v>
-                  </c:pt>
-                  <c:pt idx="91">
-                    <c:v>92</c:v>
-                  </c:pt>
-                  <c:pt idx="92">
-                    <c:v>93</c:v>
-                  </c:pt>
-                  <c:pt idx="93">
-                    <c:v>94</c:v>
-                  </c:pt>
-                  <c:pt idx="94">
-                    <c:v>95</c:v>
-                  </c:pt>
-                  <c:pt idx="95">
-                    <c:v>96</c:v>
-                  </c:pt>
-                  <c:pt idx="96">
-                    <c:v>97</c:v>
-                  </c:pt>
-                  <c:pt idx="97">
-                    <c:v>98</c:v>
-                  </c:pt>
-                  <c:pt idx="98">
-                    <c:v>99</c:v>
-                  </c:pt>
-                  <c:pt idx="99">
-                    <c:v>100</c:v>
-                  </c:pt>
-                  <c:pt idx="100">
-                    <c:v>101</c:v>
-                  </c:pt>
-                  <c:pt idx="101">
-                    <c:v>102</c:v>
-                  </c:pt>
-                  <c:pt idx="102">
-                    <c:v>103</c:v>
-                  </c:pt>
-                  <c:pt idx="103">
-                    <c:v>104</c:v>
-                  </c:pt>
-                  <c:pt idx="104">
-                    <c:v>105</c:v>
-                  </c:pt>
-                  <c:pt idx="105">
-                    <c:v>106</c:v>
-                  </c:pt>
-                  <c:pt idx="106">
-                    <c:v>107</c:v>
-                  </c:pt>
-                  <c:pt idx="107">
-                    <c:v>108</c:v>
-                  </c:pt>
-                  <c:pt idx="108">
-                    <c:v>109</c:v>
-                  </c:pt>
-                  <c:pt idx="109">
-                    <c:v>110</c:v>
-                  </c:pt>
-                  <c:pt idx="110">
-                    <c:v>111</c:v>
-                  </c:pt>
-                  <c:pt idx="111">
-                    <c:v>112</c:v>
-                  </c:pt>
-                  <c:pt idx="112">
-                    <c:v>113</c:v>
-                  </c:pt>
-                  <c:pt idx="113">
-                    <c:v>114</c:v>
-                  </c:pt>
-                  <c:pt idx="114">
-                    <c:v>115</c:v>
-                  </c:pt>
-                  <c:pt idx="115">
-                    <c:v>116</c:v>
-                  </c:pt>
-                  <c:pt idx="116">
-                    <c:v>117</c:v>
-                  </c:pt>
-                  <c:pt idx="117">
-                    <c:v>118</c:v>
-                  </c:pt>
-                  <c:pt idx="118">
-                    <c:v>119</c:v>
-                  </c:pt>
-                  <c:pt idx="119">
-                    <c:v>120</c:v>
-                  </c:pt>
-                  <c:pt idx="120">
-                    <c:v>121</c:v>
-                  </c:pt>
-                  <c:pt idx="121">
-                    <c:v>122</c:v>
-                  </c:pt>
-                  <c:pt idx="122">
-                    <c:v>123</c:v>
-                  </c:pt>
-                  <c:pt idx="123">
-                    <c:v>124</c:v>
-                  </c:pt>
-                  <c:pt idx="124">
-                    <c:v>125</c:v>
-                  </c:pt>
-                  <c:pt idx="125">
-                    <c:v>126</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>126</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Report!$I$38:$I$163</c:f>
+              <c:f>[0]!_VN1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="126"/>
@@ -1700,7 +1324,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Report!$H$38:$H$293</c:f>
+              <c:f>[0]!_TFW1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="256"/>
@@ -3295,7 +2919,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Report!$H$38:$H$221</c:f>
+              <c:f>[0]!_TFW2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="184"/>
@@ -4458,10 +4082,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Report!$H$38:$H$290</c:f>
+              <c:f>[0]!_TLT1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="253"/>
+                <c:ptCount val="273"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -5220,6 +4844,66 @@
                 </c:pt>
                 <c:pt idx="252">
                   <c:v>253</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>254</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>257</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>258</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>259</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>261</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>262</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>263</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>264</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>266</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>267</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>268</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>269</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>271</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>272</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>273</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6035,7 +5719,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Report!$H$38:$H$310</c:f>
+              <c:f>[0]!_TLT2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="273"/>
@@ -13633,7 +13317,7 @@
   <dimension ref="A1:Q1165"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T12" sqref="T12"/>
+      <selection activeCell="T21" sqref="T21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -13727,31 +13411,31 @@
     </row>
     <row r="33" spans="2:17" x14ac:dyDescent="0.25">
       <c r="I33">
-        <f>COUNTA(_xlfn.ANCHORARRAY(I38))</f>
+        <f t="shared" ref="I33:O33" si="0">COUNTA(_xlfn.ANCHORARRAY(I38))</f>
         <v>126</v>
       </c>
       <c r="J33">
-        <f>COUNTA(_xlfn.ANCHORARRAY(J38))</f>
+        <f t="shared" si="0"/>
         <v>256</v>
       </c>
       <c r="K33">
-        <f>COUNTA(_xlfn.ANCHORARRAY(K38))</f>
+        <f t="shared" si="0"/>
         <v>184</v>
       </c>
       <c r="L33">
-        <f>COUNTA(_xlfn.ANCHORARRAY(L38))</f>
+        <f t="shared" si="0"/>
         <v>253</v>
       </c>
       <c r="M33">
-        <f>COUNTA(_xlfn.ANCHORARRAY(M38))</f>
+        <f t="shared" si="0"/>
         <v>273</v>
       </c>
       <c r="N33">
-        <f>COUNTA(_xlfn.ANCHORARRAY(N38))</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="O33">
-        <f>COUNTA(_xlfn.ANCHORARRAY(O38))</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
     </row>

</xml_diff>